<commit_message>
adding position to xlsx
</commit_message>
<xml_diff>
--- a/src/lib/test.xlsx
+++ b/src/lib/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tim.kershaw\oflog-automated-text\src\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8F0BCB-4276-4345-990B-A48DE407A2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BC1D99-ABE0-4F29-AFD8-7AE34EE85C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14505" xr2:uid="{D19ADD91-E08A-4880-A6B4-AC16BCE7FEC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="24">
   <si>
     <t>topic</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>penultimateValue</t>
+  </si>
+  <si>
+    <t>position</t>
   </si>
 </sst>
 </file>
@@ -148,8 +151,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -486,15 +489,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0000E9-2B9C-48FF-98BB-322E6A2B8C83}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I30"/>
+      <selection activeCell="D22" sqref="D22:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,25 +508,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -533,26 +539,30 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
+      <c r="D2" s="1" t="str">
+        <f>_xlfn.CONCAT(C2,"_",B2)</f>
+        <v>ASC1_1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>7.5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -562,26 +572,30 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
+      <c r="D3" s="1" t="str">
+        <f t="shared" ref="D3:D10" si="0">_xlfn.CONCAT(C3,"_",B3)</f>
+        <v>ASC1_1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2">
-        <v>3</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
         <v>7.5</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -591,26 +605,30 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASC1_1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>1.5</v>
       </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -620,26 +638,30 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASC1_1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>0.5</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>1.5</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -649,26 +671,30 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASC1_1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>-0.5</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>0.5</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -678,24 +704,28 @@
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASC1_1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>-1.5</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>-0.5</v>
       </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -705,24 +735,28 @@
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASC1_1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>-3</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>-1.5</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -732,24 +766,28 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASC1_1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>-7.5</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>-3</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -759,35 +797,40 @@
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASC1_1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>-7.5</v>
       </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -797,24 +840,28 @@
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
+      <c r="D12" s="1" t="str">
+        <f>_xlfn.CONCAT(C12,"_",B12)</f>
+        <v>ASC1_2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>7.5</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -824,24 +871,28 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
+      <c r="D13" s="1" t="str">
+        <f t="shared" ref="D13:D20" si="1">_xlfn.CONCAT(C13,"_",B13)</f>
+        <v>ASC1_2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="2">
-        <v>3</v>
-      </c>
-      <c r="H13" s="1">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1">
         <v>7.5</v>
       </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -851,24 +902,28 @@
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ASC1_2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="2">
         <v>1.5</v>
       </c>
-      <c r="H14" s="2">
-        <v>3</v>
-      </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -878,26 +933,30 @@
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ASC1_2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="2">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="2">
         <v>0.5</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>1.5</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -907,24 +966,28 @@
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ASC1_2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="2">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="2">
         <v>-0.5</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>0.5</v>
       </c>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -934,24 +997,28 @@
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ASC1_2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="2">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="2">
         <v>-1.5</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>-0.5</v>
       </c>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -961,24 +1028,28 @@
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ASC1_2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="2">
+        <v>12</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="2">
         <v>-3</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>-1.5</v>
       </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -988,24 +1059,28 @@
       <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ASC1_2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="2">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="2">
         <v>-7.5</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>-3</v>
       </c>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1015,24 +1090,28 @@
       <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
+      <c r="D20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ASC1_2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>-7.5</v>
       </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1042,8 +1121,9 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1053,24 +1133,28 @@
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
+      <c r="D22" s="1" t="str">
+        <f>_xlfn.CONCAT(C22,"_",B22)</f>
+        <v>ASC1_3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>7.5</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1080,24 +1164,28 @@
       <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>11</v>
+      <c r="D23" s="1" t="str">
+        <f t="shared" ref="D23:D30" si="2">_xlfn.CONCAT(C23,"_",B23)</f>
+        <v>ASC1_3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="2">
-        <v>3</v>
-      </c>
-      <c r="H23" s="1">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1">
         <v>7.5</v>
       </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1107,24 +1195,28 @@
       <c r="C24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>11</v>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ASC1_3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="2">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="2">
         <v>1.5</v>
       </c>
-      <c r="H24" s="2">
-        <v>3</v>
-      </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1134,24 +1226,28 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>11</v>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ASC1_3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="2">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="2">
         <v>0.5</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>1.5</v>
       </c>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1161,24 +1257,28 @@
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>11</v>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ASC1_3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="2">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2">
         <v>-0.5</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>0.5</v>
       </c>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1188,24 +1288,28 @@
       <c r="C27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>11</v>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ASC1_3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="2">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="2">
         <v>-1.5</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>-0.5</v>
       </c>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -1215,24 +1319,28 @@
       <c r="C28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ASC1_3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="2">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="2">
         <v>-3</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>-1.5</v>
       </c>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1242,24 +1350,28 @@
       <c r="C29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>11</v>
+      <c r="D29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ASC1_3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="2">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="2">
         <v>-7.5</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>-3</v>
       </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -1269,22 +1381,26 @@
       <c r="C30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
+      <c r="D30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ASC1_3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>-7.5</v>
       </c>
-      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added text to map excel
</commit_message>
<xml_diff>
--- a/src/lib/test.xlsx
+++ b/src/lib/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tim.kershaw\oflog-automated-text\src\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BC1D99-ABE0-4F29-AFD8-7AE34EE85C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B32CAE-50FB-4898-864B-5BA6115F4550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14505" xr2:uid="{D19ADD91-E08A-4880-A6B4-AC16BCE7FEC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D19ADD91-E08A-4880-A6B4-AC16BCE7FEC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="27">
   <si>
     <t>topic</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>position</t>
+  </si>
+  <si>
+    <t>slightly lower</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>much lower</t>
   </si>
 </sst>
 </file>
@@ -492,7 +501,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D30"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +732,9 @@
       <c r="I7" s="2">
         <v>-0.5</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -754,7 +765,9 @@
       <c r="I8" s="2">
         <v>-1.5</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -785,7 +798,9 @@
       <c r="I9" s="2">
         <v>-3</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -816,7 +831,9 @@
       <c r="I10" s="1">
         <v>-7.5</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
risky text change - any breaks due to Word doc
</commit_message>
<xml_diff>
--- a/src/lib/test.xlsx
+++ b/src/lib/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tim.kershaw\oflog-automated-text\src\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C074B08-2E45-4737-A61F-B091B7FC47A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C053C1-1F41-4C10-82B4-9B978581EAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14505" xr2:uid="{D19ADD91-E08A-4880-A6B4-AC16BCE7FEC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="26">
   <si>
     <t>topic</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>much lower than</t>
+  </si>
+  <si>
+    <t>ASC2</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0000E9-2B9C-48FF-98BB-322E6A2B8C83}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,6 +1447,921 @@
         <v>-7.5</v>
       </c>
       <c r="J30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1" t="str">
+        <f>_xlfn.CONCAT(C32,"_",B32)</f>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1" t="str">
+        <f t="shared" ref="D33:D40" si="3">_xlfn.CONCAT(C33,"_",B33)</f>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="2">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I34" s="2">
+        <v>3</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="I37" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="2">
+        <v>-3</v>
+      </c>
+      <c r="I38" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="2">
+        <v>-7.5</v>
+      </c>
+      <c r="I39" s="2">
+        <v>-3</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ASC2_1</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="I40" s="1">
+        <v>-7.5</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="1" t="str">
+        <f>_xlfn.CONCAT(C42,"_",B42)</f>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I42" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="1" t="str">
+        <f t="shared" ref="D43:D50" si="4">_xlfn.CONCAT(C43,"_",B43)</f>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="2">
+        <v>3</v>
+      </c>
+      <c r="I43" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I44" s="2">
+        <v>3</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="I47" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="2">
+        <v>-3</v>
+      </c>
+      <c r="I48" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="2">
+        <v>-7.5</v>
+      </c>
+      <c r="I49" s="2">
+        <v>-3</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ASC2_2</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="I50" s="1">
+        <v>-7.5</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <f>_xlfn.CONCAT(C52,"_",B52)</f>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I52" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="1">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <f t="shared" ref="D53:D60" si="5">_xlfn.CONCAT(C53,"_",B53)</f>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="2">
+        <v>3</v>
+      </c>
+      <c r="I53" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I54" s="2">
+        <v>3</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="1">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="1">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="1">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="I57" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="1">
+        <v>3</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H58" s="2">
+        <v>-3</v>
+      </c>
+      <c r="I58" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="1">
+        <v>3</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="2">
+        <v>-7.5</v>
+      </c>
+      <c r="I59" s="2">
+        <v>-3</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="1">
+        <v>3</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>ASC2_3</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="I60" s="1">
+        <v>-7.5</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
potentially breaking changes to MS docs
</commit_message>
<xml_diff>
--- a/src/lib/test.xlsx
+++ b/src/lib/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tim.kershaw\oflog-automated-text\src\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C053C1-1F41-4C10-82B4-9B978581EAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF23FCBA-E8C6-4158-A83A-C44CE9C0E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14505" xr2:uid="{D19ADD91-E08A-4880-A6B4-AC16BCE7FEC7}"/>
   </bookViews>
@@ -113,7 +113,7 @@
     <t>much lower than</t>
   </si>
   <si>
-    <t>ASC2</t>
+    <t>ASC4</t>
   </si>
 </sst>
 </file>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0000E9-2B9C-48FF-98BB-322E6A2B8C83}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1207,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" s="2">
         <v>3</v>
@@ -1240,7 +1240,7 @@
         <v>12</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H24" s="2">
         <v>1.5</v>
@@ -1273,7 +1273,7 @@
         <v>12</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" s="2">
         <v>0.5</v>
@@ -1306,7 +1306,7 @@
         <v>12</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" s="2">
         <v>-0.5</v>
@@ -1339,7 +1339,7 @@
         <v>12</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H27" s="2">
         <v>-1.5</v>
@@ -1372,7 +1372,7 @@
         <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H28" s="2">
         <v>-3</v>
@@ -1405,7 +1405,7 @@
         <v>12</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" s="2">
         <v>-7.5</v>
@@ -1438,7 +1438,7 @@
         <v>12</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H30" s="2">
         <v>-1000</v>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="D32" s="1" t="str">
         <f>_xlfn.CONCAT(C32,"_",B32)</f>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>11</v>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D33" s="1" t="str">
         <f t="shared" ref="D33:D40" si="3">_xlfn.CONCAT(C33,"_",B33)</f>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>11</v>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="D34" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>11</v>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="D35" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>11</v>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="D36" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>11</v>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D37" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>11</v>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="D38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>11</v>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="D39" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>11</v>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="D40" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ASC2_1</v>
+        <v>ASC4_1</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>11</v>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D42" s="1" t="str">
         <f>_xlfn.CONCAT(C42,"_",B42)</f>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>11</v>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="D43" s="1" t="str">
         <f t="shared" ref="D43:D50" si="4">_xlfn.CONCAT(C43,"_",B43)</f>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>11</v>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D44" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>11</v>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="D45" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>11</v>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D46" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>11</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="D47" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>11</v>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>11</v>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="D49" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>11</v>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ASC2_2</v>
+        <v>ASC4_2</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>11</v>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="D52" s="1" t="str">
         <f>_xlfn.CONCAT(C52,"_",B52)</f>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>11</v>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="D53" s="1" t="str">
         <f t="shared" ref="D53:D60" si="5">_xlfn.CONCAT(C53,"_",B53)</f>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>11</v>
@@ -2122,7 +2122,7 @@
         <v>12</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H53" s="2">
         <v>3</v>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>11</v>
@@ -2155,7 +2155,7 @@
         <v>12</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H54" s="2">
         <v>1.5</v>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="D55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>11</v>
@@ -2188,7 +2188,7 @@
         <v>12</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H55" s="2">
         <v>0.5</v>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="D56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>11</v>
@@ -2221,7 +2221,7 @@
         <v>12</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H56" s="2">
         <v>-0.5</v>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="D57" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>11</v>
@@ -2254,7 +2254,7 @@
         <v>12</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H57" s="2">
         <v>-1.5</v>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="D58" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
@@ -2287,7 +2287,7 @@
         <v>12</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H58" s="2">
         <v>-3</v>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="D59" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>11</v>
@@ -2320,7 +2320,7 @@
         <v>12</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H59" s="2">
         <v>-7.5</v>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="D60" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>ASC2_3</v>
+        <v>ASC4_3</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>11</v>
@@ -2353,7 +2353,7 @@
         <v>12</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H60" s="2">
         <v>-1000</v>

</xml_diff>